<commit_message>
Label and ASN for chewy are done!
</commit_message>
<xml_diff>
--- a/Finished/Chewy/Chewy 856 ASN PO RS41260550 10.02.2024.xlsx
+++ b/Finished/Chewy/Chewy 856 ASN PO RS41260550 10.02.2024.xlsx
@@ -1305,7 +1305,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1399,7 +1399,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1540,7 +1540,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1634,7 +1634,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">

</xml_diff>